<commit_message>
Liederupdate + Fortschritt updated
</commit_message>
<xml_diff>
--- a/Fortschritt.xlsx
+++ b/Fortschritt.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leopold Fajtak\Documents\GitHub\cantuspruegel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastianecker/DanubiaGithub/cantuspruegel/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13695" yWindow="3165" windowWidth="27765" windowHeight="16245" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="96">
   <si>
     <t>Liedname</t>
   </si>
@@ -320,7 +320,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -367,7 +367,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -647,13 +647,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="D92" sqref="D92"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="46.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -675,7 +675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -714,9 +714,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -728,6 +734,12 @@
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="B11" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -763,82 +775,88 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
@@ -853,7 +871,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
@@ -868,12 +886,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
@@ -888,12 +906,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
@@ -908,17 +926,17 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>47</v>
       </c>
@@ -928,7 +946,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>49</v>
       </c>
@@ -957,12 +975,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>54</v>
       </c>
@@ -972,7 +990,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>56</v>
       </c>
@@ -991,7 +1009,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>58</v>
       </c>
@@ -1001,12 +1019,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>61</v>
       </c>
@@ -1025,7 +1043,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>63</v>
       </c>
@@ -1035,7 +1053,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>65</v>
       </c>
@@ -1080,7 +1098,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>74</v>
       </c>
@@ -1090,7 +1108,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>76</v>
       </c>
@@ -1105,7 +1123,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>79</v>
       </c>
@@ -1119,13 +1137,19 @@
       <c r="A82" s="1" t="s">
         <v>81</v>
       </c>
+      <c r="B82" t="s">
+        <v>92</v>
+      </c>
+      <c r="C82" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>83</v>
       </c>
@@ -1145,12 +1169,12 @@
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>88</v>
       </c>

</xml_diff>

<commit_message>
4 Offizlieder + Fortschritt update
</commit_message>
<xml_diff>
--- a/Fortschritt.xlsx
+++ b/Fortschritt.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="98">
   <si>
     <t>Liedname</t>
   </si>
@@ -315,6 +315,12 @@
   </si>
   <si>
     <t>verweis</t>
+  </si>
+  <si>
+    <t>Lhymnen</t>
+  </si>
+  <si>
+    <t>Offizium</t>
   </si>
 </sst>
 </file>
@@ -647,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -799,6 +805,12 @@
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="B21" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
@@ -809,6 +821,12 @@
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="B23" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
@@ -825,6 +843,12 @@
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="B25" t="s">
+        <v>96</v>
+      </c>
+      <c r="C25" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
@@ -861,82 +885,106 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>97</v>
+      </c>
+      <c r="C37" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>96</v>
+      </c>
+      <c r="C38" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>96</v>
+      </c>
+      <c r="C39" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>47</v>
       </c>
@@ -979,11 +1027,23 @@
       <c r="A54" s="1" t="s">
         <v>53</v>
       </c>
+      <c r="B54" t="s">
+        <v>96</v>
+      </c>
+      <c r="C54" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="B55" t="s">
+        <v>96</v>
+      </c>
+      <c r="C55" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
@@ -1023,6 +1083,12 @@
       <c r="A61" s="1" t="s">
         <v>60</v>
       </c>
+      <c r="B61" t="s">
+        <v>96</v>
+      </c>
+      <c r="C61" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
@@ -1048,82 +1114,88 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>97</v>
+      </c>
+      <c r="C77" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>79</v>
       </c>
@@ -1177,6 +1249,12 @@
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>88</v>
+      </c>
+      <c r="B89" t="s">
+        <v>96</v>
+      </c>
+      <c r="C89" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Neue Lieder + Fortschritt update
</commit_message>
<xml_diff>
--- a/Fortschritt.xlsx
+++ b/Fortschritt.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17030"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastianecker/DanubiaGithub/cantuspruegel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\Documents\GitHub\cantuspruegel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="99">
   <si>
     <t>Liedname</t>
   </si>
@@ -321,12 +321,15 @@
   </si>
   <si>
     <t>Offizium</t>
+  </si>
+  <si>
+    <t>Officium</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -373,7 +376,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -654,15 +657,15 @@
   <dimension ref="A1:D91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -676,17 +679,23 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -700,27 +709,27 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -731,12 +740,12 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -747,17 +756,23 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>98</v>
+      </c>
+      <c r="C12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -771,53 +786,53 @@
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
-        <v>97</v>
-      </c>
-      <c r="C21" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -828,7 +843,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -839,7 +854,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -850,79 +865,85 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>98</v>
+      </c>
+      <c r="C28" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C33" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C37" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
@@ -933,7 +954,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
@@ -954,12 +975,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
@@ -973,18 +994,24 @@
       <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>98</v>
+      </c>
+      <c r="C45" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>47</v>
       </c>
@@ -994,7 +1021,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>49</v>
       </c>
@@ -1023,7 +1050,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>53</v>
       </c>
@@ -1034,7 +1061,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>54</v>
       </c>
@@ -1050,7 +1077,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>56</v>
       </c>
@@ -1069,7 +1096,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>58</v>
       </c>
@@ -1079,7 +1106,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>60</v>
       </c>
@@ -1090,7 +1117,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>61</v>
       </c>
@@ -1109,7 +1136,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>63</v>
       </c>
@@ -1119,7 +1146,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>65</v>
       </c>
@@ -1164,7 +1191,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>74</v>
       </c>
@@ -1174,7 +1201,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>76</v>
       </c>
@@ -1195,7 +1222,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>79</v>
       </c>
@@ -1221,7 +1248,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>83</v>
       </c>
@@ -1241,12 +1268,12 @@
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>88</v>
       </c>

</xml_diff>

<commit_message>
Inoffizlieder + Kursivmakro + Fortschritt update
</commit_message>
<xml_diff>
--- a/Fortschritt.xlsx
+++ b/Fortschritt.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="131">
   <si>
     <t>Liedname</t>
   </si>
@@ -417,6 +417,9 @@
   </si>
   <si>
     <t>Lasset die feurigen Bomben erschallen</t>
+  </si>
+  <si>
+    <t>Inofficium</t>
   </si>
 </sst>
 </file>
@@ -755,10 +758,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D121"/>
+  <dimension ref="A1:D120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="B121" activeCellId="27" sqref="B3 B6 B15 B17 B18 B20:B22 B27:B28 B30:B32 B36 B42 B44 B49 B51:B53 B60 B69 B73 B75 B79 B81:B83 B85 B87 B89:B90 B95 B104 B108:B109 B111 B113:B114 B121"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -766,7 +769,7 @@
     <col min="1" max="1" width="46.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -811,7 +814,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="C6" t="s">
         <v>93</v>
@@ -846,26 +849,32 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>120</v>
+      <c r="A12" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>7</v>
+      <c r="A13" s="3" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>115</v>
+      <c r="A14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>92</v>
+        <v>130</v>
       </c>
       <c r="C15" t="s">
         <v>93</v>
@@ -873,15 +882,21 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="C17" t="s">
         <v>93</v>
@@ -889,10 +904,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
       <c r="C18" t="s">
         <v>93</v>
@@ -900,26 +915,32 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="B19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" t="s">
+        <v>93</v>
+      </c>
+      <c r="D19" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="C20" t="s">
         <v>93</v>
-      </c>
-      <c r="D20" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B21" t="s">
         <v>98</v>
@@ -930,38 +951,38 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22" t="s">
-        <v>98</v>
-      </c>
-      <c r="C22" t="s">
-        <v>93</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="B26" t="s">
+        <v>98</v>
+      </c>
+      <c r="C26" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B27" t="s">
         <v>98</v>
@@ -971,27 +992,27 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B28" t="s">
-        <v>98</v>
-      </c>
-      <c r="C28" t="s">
-        <v>93</v>
+      <c r="A28" s="3" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>116</v>
+      <c r="A29" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B30" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C30" t="s">
         <v>93</v>
@@ -999,146 +1020,164 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B31" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C31" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B32" t="s">
-        <v>96</v>
-      </c>
-      <c r="C32" t="s">
-        <v>93</v>
+      <c r="A32" s="3" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>108</v>
+      <c r="A33" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" t="s">
+        <v>130</v>
+      </c>
+      <c r="C33" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="B35" t="s">
+        <v>98</v>
+      </c>
+      <c r="C35" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B36" t="s">
-        <v>98</v>
-      </c>
-      <c r="C36" t="s">
-        <v>93</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>29</v>
+      <c r="A38" s="3" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>107</v>
+      <c r="A41" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B41" t="s">
+        <v>98</v>
+      </c>
+      <c r="C41" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B42" t="s">
-        <v>98</v>
-      </c>
-      <c r="C42" t="s">
-        <v>93</v>
+        <v>31</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="B43" t="s">
+        <v>98</v>
+      </c>
+      <c r="C43" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B44" t="s">
-        <v>98</v>
-      </c>
-      <c r="C44" t="s">
-        <v>93</v>
+      <c r="A44" s="3" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
-        <v>110</v>
+      <c r="A45" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B45" t="s">
+        <v>130</v>
+      </c>
+      <c r="C45" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>33</v>
+      <c r="A46" s="3" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>128</v>
+      <c r="A47" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B47" t="s">
+        <v>130</v>
+      </c>
+      <c r="C47" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="B48" t="s">
+        <v>98</v>
+      </c>
+      <c r="C48" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B49" t="s">
-        <v>98</v>
-      </c>
-      <c r="C49" t="s">
-        <v>93</v>
+      <c r="A49" s="3" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
-        <v>114</v>
+      <c r="A50" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B50" t="s">
+        <v>98</v>
+      </c>
+      <c r="C50" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B51" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C51" t="s">
         <v>93</v>
@@ -1146,7 +1185,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B52" t="s">
         <v>96</v>
@@ -1157,192 +1196,198 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B53" t="s">
-        <v>96</v>
-      </c>
-      <c r="C53" t="s">
-        <v>93</v>
+        <v>39</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>40</v>
+      <c r="A55" s="3" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
-        <v>123</v>
+      <c r="A56" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+      <c r="B59" t="s">
+        <v>98</v>
+      </c>
+      <c r="C59" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B60" t="s">
-        <v>98</v>
-      </c>
-      <c r="C60" t="s">
-        <v>93</v>
+      <c r="A60" s="3" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="3" t="s">
-        <v>109</v>
+      <c r="A62" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
-        <v>45</v>
+      <c r="A63" s="3" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="3" t="s">
-        <v>103</v>
+      <c r="A64" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B64" t="s">
+        <v>130</v>
+      </c>
+      <c r="C64" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
-        <v>48</v>
+      <c r="A67" s="3" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="3" t="s">
-        <v>113</v>
+      <c r="A68" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B68" t="s">
+        <v>99</v>
+      </c>
+      <c r="C68" t="s">
+        <v>93</v>
+      </c>
+      <c r="D68" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B69" t="s">
-        <v>92</v>
-      </c>
-      <c r="C69" t="s">
-        <v>93</v>
-      </c>
-      <c r="D69" t="s">
-        <v>95</v>
+        <v>50</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
+      </c>
+      <c r="B72" t="s">
+        <v>96</v>
+      </c>
+      <c r="C72" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B73" t="s">
+      <c r="A73" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B74" t="s">
         <v>96</v>
       </c>
-      <c r="C73" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="3" t="s">
-        <v>129</v>
+      <c r="C74" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B75" t="s">
-        <v>96</v>
-      </c>
-      <c r="C75" t="s">
-        <v>93</v>
+        <v>55</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
-        <v>55</v>
+      <c r="A76" s="3" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="3" t="s">
-        <v>122</v>
+      <c r="A77" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
+      </c>
+      <c r="B78" t="s">
+        <v>92</v>
+      </c>
+      <c r="C78" t="s">
+        <v>93</v>
+      </c>
+      <c r="D78" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B79" t="s">
-        <v>92</v>
-      </c>
-      <c r="C79" t="s">
-        <v>93</v>
-      </c>
-      <c r="D79" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
+      </c>
+      <c r="B80" t="s">
+        <v>98</v>
+      </c>
+      <c r="C80" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B81" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C81" t="s">
         <v>93</v>
@@ -1350,69 +1395,69 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B82" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C82" t="s">
         <v>93</v>
+      </c>
+      <c r="D82" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B83" t="s">
-        <v>92</v>
-      </c>
-      <c r="C83" t="s">
-        <v>93</v>
-      </c>
-      <c r="D83" t="s">
-        <v>95</v>
+        <v>62</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>62</v>
+        <v>94</v>
+      </c>
+      <c r="B84" t="s">
+        <v>92</v>
+      </c>
+      <c r="C84" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B85" t="s">
-        <v>92</v>
-      </c>
-      <c r="C85" t="s">
-        <v>93</v>
+      <c r="A85" s="3" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="3" t="s">
-        <v>124</v>
+      <c r="A86" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B86" t="s">
+        <v>98</v>
+      </c>
+      <c r="C86" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B87" t="s">
-        <v>98</v>
-      </c>
-      <c r="C87" t="s">
-        <v>93</v>
+      <c r="A87" s="3" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="3" t="s">
-        <v>106</v>
+      <c r="A88" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B88" t="s">
+        <v>98</v>
+      </c>
+      <c r="C88" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
-        <v>64</v>
+      <c r="A89" t="s">
+        <v>100</v>
       </c>
       <c r="B89" t="s">
         <v>98</v>
@@ -1422,119 +1467,131 @@
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>100</v>
-      </c>
-      <c r="B90" t="s">
-        <v>98</v>
-      </c>
-      <c r="C90" t="s">
-        <v>93</v>
+      <c r="A90" s="3" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="3" t="s">
-        <v>126</v>
+      <c r="A94" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B94" t="s">
+        <v>98</v>
+      </c>
+      <c r="C94" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B95" t="s">
-        <v>98</v>
-      </c>
-      <c r="C95" t="s">
-        <v>93</v>
+        <v>66</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
+      </c>
+      <c r="B98" t="s">
+        <v>130</v>
+      </c>
+      <c r="C98" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
-        <v>70</v>
+      <c r="A100" s="3" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="3" t="s">
-        <v>101</v>
+      <c r="A101" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="B102" t="s">
+        <v>130</v>
+      </c>
+      <c r="C102" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
+      </c>
+      <c r="B103" t="s">
+        <v>98</v>
+      </c>
+      <c r="C103" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B104" t="s">
-        <v>98</v>
-      </c>
-      <c r="C104" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" s="1" t="s">
-        <v>75</v>
+      <c r="A106" s="3" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" s="3" t="s">
-        <v>104</v>
+      <c r="A107" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B107" t="s">
+        <v>97</v>
+      </c>
+      <c r="C107" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B108" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C108" t="s">
         <v>93</v>
@@ -1542,96 +1599,91 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B109" t="s">
-        <v>98</v>
-      </c>
-      <c r="C109" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
+      </c>
+      <c r="B110" t="s">
+        <v>98</v>
+      </c>
+      <c r="C110" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B111" t="s">
-        <v>98</v>
-      </c>
-      <c r="C111" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
+      </c>
+      <c r="B112" t="s">
+        <v>99</v>
+      </c>
+      <c r="C112" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B113" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C113" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B114" t="s">
-        <v>98</v>
-      </c>
-      <c r="C114" t="s">
-        <v>93</v>
+      <c r="A114" s="3" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="3" t="s">
-        <v>112</v>
+      <c r="A115" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
+      </c>
+      <c r="B119" t="s">
+        <v>130</v>
+      </c>
+      <c r="C119" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B121" t="s">
+      <c r="B120" t="s">
         <v>96</v>
       </c>
-      <c r="C121" t="s">
+      <c r="C120" t="s">
         <v>93</v>
       </c>
     </row>

</xml_diff>